<commit_message>
Data Cleaning and Preprocessing, notes in data folders, Google Colab folder to follow
</commit_message>
<xml_diff>
--- a/data/Data Dictionaries/reimbursements_data_dictionary.xlsx
+++ b/data/Data Dictionaries/reimbursements_data_dictionary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\RADD\RDA_Interview_Exercise\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\RADD\RDA_Interview_Exercise\data\Data Dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA9B756-43C9-4310-8B77-45B175CAD462}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54ED6716-DEB3-4D67-B344-D729E7E9F1AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="-16155" windowWidth="14010" windowHeight="15630" xr2:uid="{4D544137-E322-4594-8770-66637C88F31A}"/>
   </bookViews>
@@ -121,20 +121,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Primary spoken languages of the individuals on a given </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color theme="1"/>
-        <rFont val="Ubuntu Mono"/>
-        <family val="3"/>
-      </rPr>
-      <t>CaseID</t>
-    </r>
-  </si>
-  <si>
     <t>County of residence of all individuals associated with a given case.</t>
   </si>
   <si>
@@ -148,6 +134,9 @@
   </si>
   <si>
     <t>Date that the reimbursement payment to the theft victim was processed.</t>
+  </si>
+  <si>
+    <t>Primary spoken languages of the individuals on a given CaseID</t>
   </si>
 </sst>
 </file>
@@ -536,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD679047-F6E4-4D39-819E-7732CE178C8D}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,7 +534,7 @@
     <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" customFormat="1" ht="30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -601,15 +590,15 @@
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="118.2" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="120" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="150" x14ac:dyDescent="0.35">
@@ -617,7 +606,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="135" x14ac:dyDescent="0.35">
@@ -625,7 +614,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="135" x14ac:dyDescent="0.35">
@@ -633,7 +622,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="165" x14ac:dyDescent="0.35">
@@ -641,7 +630,7 @@
         <v>19</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>